<commit_message>
correções para novos requisitos
</commit_message>
<xml_diff>
--- a/docs/Requisitos.xlsx
+++ b/docs/Requisitos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>Número</t>
   </si>
@@ -34,34 +34,34 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>Perfis de Usuários: cadastro e edição de informações pessoais e acadêmicas (curso, período, disciplinas).</t>
+    <t>Perfis de Usuário – Permitir cadastro, edição e personalização de perfis com diferentes papéis e controle de privacidade.</t>
   </si>
   <si>
     <t>R-02</t>
   </si>
   <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Upload de foto e personalização do perfil.</t>
+    <t>Cadastro e Administração – Gerenciar fluxo de cadastro e aprovações por painel administrativo.</t>
   </si>
   <si>
     <t>R-03</t>
   </si>
   <si>
-    <t>Exibição de histórico de atividades dentro da plataforma (postagens, grupos, eventos).</t>
+    <t>Feed Principal – Publicar e interagir com conteúdos categorizados, priorizando avisos e posts relevantes.</t>
   </si>
   <si>
     <t>R-04</t>
   </si>
   <si>
-    <t>Configurações de privacidade (controle de quem pode visualizar informações).</t>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Eventos Universitários – Criar, divulgar e gerenciar inscrições e lembretes de eventos acadêmicos e culturais.</t>
   </si>
   <si>
     <t>R-05</t>
   </si>
   <si>
-    <t>Feed de Notícias: publicação de textos, imagens, vídeos e links.</t>
+    <t>Mensagens e Comunicação – Trocar mensagens individuais e em grupo com suporte a mídia e notificações.</t>
   </si>
   <si>
     <t>R-06</t>
@@ -70,13 +70,13 @@
     <t>Baixa</t>
   </si>
   <si>
-    <t>Interações no feed: curtidas, comentários e compartilhamentos internos.</t>
+    <t>Sistema de Notificações – Enviar alertas sobre posts, eventos e mensagens, personalizáveis pelo usuário.</t>
   </si>
   <si>
     <t>R-07</t>
   </si>
   <si>
-    <t>Algoritmo de relevância baseado em interações e interesses acadêmicos.</t>
+    <t>Busca e Descoberta – Buscar e sugerir usuários, cursos, grupos e eventos com base em afinidades.</t>
   </si>
   <si>
     <t>R-08</t>
@@ -88,106 +88,52 @@
     <t>R-09</t>
   </si>
   <si>
-    <t>Grupos de Estudo: criação e gerenciamento de grupos (abertos, fechados, privados).</t>
+    <t>Moderação e Segurança – Denunciar, bloquear e revisar conteúdos e usuários com políticas de moderação.</t>
   </si>
   <si>
     <t>R-10</t>
   </si>
   <si>
-    <t>Compartilhamento de materiais (PDFs, apresentações, links).</t>
+    <t>Não Funcional</t>
+  </si>
+  <si>
+    <t>Escalabilidade – Suportar crescimento de usuários e cargas de forma eficiente.</t>
   </si>
   <si>
     <t>R-11</t>
   </si>
   <si>
-    <t xml:space="preserve">Espaço de fórum para debates e perguntas. </t>
+    <t>Segurança – Garantir proteção de dados e conformidade com LGPD.</t>
   </si>
   <si>
     <t>R-12</t>
   </si>
   <si>
-    <t>Subgrupos para disciplinas/projetos.</t>
+    <t>Usabilidade – Interface responsiva, intuitiva e acessível.</t>
   </si>
   <si>
     <t>R-13</t>
   </si>
   <si>
-    <t>Eventos: calendário, inscrições, lembretes e gerenciamento.</t>
+    <t>Desempenho – Responder a requisições rapidamente, com tempo inferior a 2 segundos.</t>
   </si>
   <si>
     <t>R-14</t>
   </si>
   <si>
-    <t>Mensagens e Comunicação: chat individual e em grupo, envio de arquivos e indicadores de presença/online.</t>
+    <t>Disponibilidade – Manter o sistema operacional 99% do tempo.</t>
   </si>
   <si>
     <t>R-15</t>
   </si>
   <si>
-    <t>Notificações: alertas sobre novas postagens, mensagens, eventos e convites.</t>
+    <t>Compatibilidade – Funcionar em principais navegadores e dispositivos móveis.</t>
   </si>
   <si>
     <t>R-16</t>
   </si>
   <si>
-    <t>Gamificação: pontos, badges, rankings e conquistas.</t>
-  </si>
-  <si>
-    <t>R-17</t>
-  </si>
-  <si>
-    <t>Busca e Descoberta: busca por usuários, disciplinas, grupos e eventos, sugestões automáticas.</t>
-  </si>
-  <si>
-    <t>R-18</t>
-  </si>
-  <si>
-    <t>Moderação e Segurança: sistema de denúncias, bloqueio e políticas de revisão.</t>
-  </si>
-  <si>
-    <t>R-19</t>
-  </si>
-  <si>
-    <t>Não Funcional</t>
-  </si>
-  <si>
-    <t>Escalabilidade: suporte inicial para 5.000 usuários ativos com possibilidade de expansão.</t>
-  </si>
-  <si>
-    <t>R-20</t>
-  </si>
-  <si>
-    <t>Segurança: criptografia de dados em trânsito (TLS) e em repouso; conformidade com a LGPD.</t>
-  </si>
-  <si>
-    <t>R-21</t>
-  </si>
-  <si>
-    <t>Usabilidade: design responsivo (mobile-first) e compatível com padrões de acessibilidade (WCAG).</t>
-  </si>
-  <si>
-    <t>R-22</t>
-  </si>
-  <si>
-    <t>Desempenho: tempo de resposta inferior a 2s para 95% das requisições.</t>
-  </si>
-  <si>
-    <t>R-23</t>
-  </si>
-  <si>
-    <t>Disponibilidade: SLA mínimo de 99% em produção.</t>
-  </si>
-  <si>
-    <t>R-24</t>
-  </si>
-  <si>
-    <t>Compatibilidade: suportar Chrome, Firefox e Edge, além de dispositivos móveis Android e iOS.</t>
-  </si>
-  <si>
-    <t>R-25</t>
-  </si>
-  <si>
-    <t>Manutenção: código modular e documentado.</t>
+    <t>Manutenção – Facilitar atualizações e evolução contínua do sistema.</t>
   </si>
 </sst>
 </file>
@@ -529,7 +475,7 @@
     <col hidden="1" min="2" max="2" width="12.63"/>
     <col customWidth="1" min="3" max="3" width="18.13"/>
     <col customWidth="1" min="4" max="4" width="23.13"/>
-    <col customWidth="1" min="6" max="6" width="81.38"/>
+    <col customWidth="1" min="6" max="6" width="90.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -582,36 +528,36 @@
       <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>9</v>
+      <c r="E7" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>14</v>
@@ -624,8 +570,8 @@
       <c r="D9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>6</v>
+      <c r="E9" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>16</v>
@@ -652,8 +598,8 @@
       <c r="D11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>18</v>
+      <c r="E11" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>21</v>
@@ -667,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>23</v>
@@ -681,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>25</v>
@@ -692,224 +638,143 @@
         <v>26</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22">
-      <c r="C22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23">
-      <c r="C23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24">
-      <c r="C24" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25">
-      <c r="C25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26">
-      <c r="C26" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27">
-      <c r="C27" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28">
-      <c r="C28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29">
-      <c r="C29" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30">
       <c r="C30" s="1"/>
@@ -5721,51 +5586,6 @@
       <c r="D991" s="2"/>
       <c r="E991" s="3"/>
     </row>
-    <row r="992">
-      <c r="C992" s="1"/>
-      <c r="D992" s="2"/>
-      <c r="E992" s="3"/>
-    </row>
-    <row r="993">
-      <c r="C993" s="1"/>
-      <c r="D993" s="2"/>
-      <c r="E993" s="3"/>
-    </row>
-    <row r="994">
-      <c r="C994" s="1"/>
-      <c r="D994" s="2"/>
-      <c r="E994" s="3"/>
-    </row>
-    <row r="995">
-      <c r="C995" s="1"/>
-      <c r="D995" s="2"/>
-      <c r="E995" s="3"/>
-    </row>
-    <row r="996">
-      <c r="C996" s="1"/>
-      <c r="D996" s="2"/>
-      <c r="E996" s="3"/>
-    </row>
-    <row r="997">
-      <c r="C997" s="1"/>
-      <c r="D997" s="2"/>
-      <c r="E997" s="3"/>
-    </row>
-    <row r="998">
-      <c r="C998" s="1"/>
-      <c r="D998" s="2"/>
-      <c r="E998" s="3"/>
-    </row>
-    <row r="999">
-      <c r="C999" s="1"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="3"/>
-    </row>
-    <row r="1000">
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="3"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>